<commit_message>
changed DEB_* sheet slightly
</commit_message>
<xml_diff>
--- a/DEB_Fundamental_Indicators.xlsx
+++ b/DEB_Fundamental_Indicators.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10488" firstSheet="3" activeTab="6" xr2:uid="{64EC43BC-41BB-45A0-AFCE-1DAA005483CE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10488" activeTab="4" xr2:uid="{64EC43BC-41BB-45A0-AFCE-1DAA005483CE}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1045" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="349">
   <si>
     <t>Balance Sheet</t>
   </si>
@@ -1067,9 +1067,6 @@
     <t>Dividend Cover</t>
   </si>
   <si>
-    <t>indicator</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -1077,6 +1074,9 @@
   </si>
   <si>
     <t>priorImportance</t>
+  </si>
+  <si>
+    <t>feature</t>
   </si>
 </sst>
 </file>
@@ -1453,10 +1453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{858D2AEB-BB99-436F-B0A6-A83763945CAB}">
-  <dimension ref="A1:C193"/>
+  <dimension ref="A1:C199"/>
   <sheetViews>
-    <sheetView topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="A116" sqref="A116:C116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="44.21875" defaultRowHeight="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3402,6 +3402,12 @@
         <v>6</v>
       </c>
     </row>
+    <row r="199" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A199">
+        <f>193 - 27</f>
+        <v>166</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3412,7 +3418,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3425,16 +3431,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>347</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -3698,9 +3704,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B4D6F37-52C0-41CD-8836-B11CE302195D}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3712,16 +3716,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>347</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -4151,16 +4155,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>347</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -4422,10 +4426,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0476A94A-DEEE-4165-92D0-958E5327144C}">
-  <dimension ref="A1:D74"/>
+  <dimension ref="A1:D75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="D75" sqref="D75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4438,16 +4442,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>347</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -5470,6 +5474,20 @@
       </c>
       <c r="D74">
         <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D75">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -5482,7 +5500,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5495,16 +5513,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>347</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -5517,6 +5535,9 @@
       <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
@@ -5528,6 +5549,9 @@
       <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
@@ -5539,6 +5563,9 @@
       <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
@@ -5550,6 +5577,9 @@
       <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
@@ -5561,6 +5591,9 @@
       <c r="C6" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
@@ -5572,6 +5605,9 @@
       <c r="C7" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
@@ -5583,6 +5619,9 @@
       <c r="C8" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
@@ -5594,6 +5633,9 @@
       <c r="C9" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
@@ -5605,6 +5647,9 @@
       <c r="C10" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
@@ -5615,6 +5660,9 @@
       </c>
       <c r="C11" s="3" t="s">
         <v>6</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -5626,7 +5674,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FB39473-7F56-40AC-829C-3D61E35A1D28}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -5638,16 +5686,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>347</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>